<commit_message>
Adiciona extração da Drogaria Minas Mais funcionando quase 100%
</commit_message>
<xml_diff>
--- a/dadosFarmaPonte/dadosXLSX/dadosFarmaPonteSuplementos.xlsx
+++ b/dadosFarmaPonte/dadosXLSX/dadosFarmaPonteSuplementos.xlsx
@@ -2271,112 +2271,112 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Go Energy Now Gel Guarana Com Acai 30gr</t>
+          <t>Whey 100  Pote Cookies 900GR Integralmedica</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>10</v>
       </c>
       <c r="C48" t="n">
-        <v>4.82</v>
+        <v>184.44</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>25480</t>
+          <t>23838</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>4.21</v>
+        <v>161.02</v>
       </c>
       <c r="F48" t="n">
-        <v>4.34</v>
+        <v>166</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/go-energy-now-gel-guarana-com-acai-30gr/p</t>
+          <t>https://www.farmaponte.com.br/whey-100-pote-cookies-900gr-integralmedica/p</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>7899621106573</t>
+          <t>7896311766376</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Sem marca</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Whey 100  Pote Cookies 900GR Integralmedica</t>
+          <t>Isotonico Go Drink Guarana C Acai 900gr Altetica</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>184.44</v>
+        <v>47.67</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>23838</t>
+          <t>25481</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>161.02</v>
+        <v>41.61</v>
       </c>
       <c r="F49" t="n">
-        <v>166</v>
+        <v>42.9</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-100-pote-cookies-900gr-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/isotonico-go-drink-guarana-c-acai-900gr-altetica/p</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>7896311766376</t>
+          <t>7899621100618</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Sem marca</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Isotonico Go Drink Guarana C Acai 900gr Altetica</t>
+          <t>Creatina 150gr Atlas</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>10</v>
       </c>
       <c r="C50" t="n">
-        <v>47.67</v>
+        <v>75.34</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>25481</t>
+          <t>23943</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>41.61</v>
+        <v>65.78</v>
       </c>
       <c r="F50" t="n">
-        <v>42.9</v>
+        <v>67.81</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/isotonico-go-drink-guarana-c-acai-900gr-altetica/p</t>
+          <t>https://www.farmaponte.com.br/creatina-150gr-atlas/p</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>7899621100618</t>
+          <t>7899732103331</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -2388,307 +2388,307 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Creatina 150gr Atlas</t>
+          <t>Coqueteleira 1Dose Nacional Integralmedica</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>75.34</v>
+        <v>35.56</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>23943</t>
+          <t>24402</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>65.78</v>
+        <v>31.04</v>
       </c>
       <c r="F51" t="n">
-        <v>67.81</v>
+        <v>32</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/creatina-150gr-atlas/p</t>
+          <t>https://www.farmaponte.com.br/coqueteleira-1dose-nacional-integralmedica/p</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>7899732103331</t>
+          <t>7896311102297</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Sem marca</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Coqueteleira 1Dose Nacional Integralmedica</t>
+          <t>Creatina Fuel 150Gr Iridium</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>10</v>
       </c>
       <c r="C52" t="n">
-        <v>35.56</v>
+        <v>61</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>24402</t>
+          <t>23969</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>31.04</v>
+        <v>53.25</v>
       </c>
       <c r="F52" t="n">
-        <v>32</v>
+        <v>54.9</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/coqueteleira-1dose-nacional-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/creatina-fuel-150gr-iridium/p</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>7896311102297</t>
+          <t>7899732113873</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Iridium</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Creatina Fuel 150Gr Iridium</t>
+          <t>Creatina 90Gr Atlas</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>10</v>
       </c>
       <c r="C53" t="n">
-        <v>61</v>
+        <v>56.56</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>23969</t>
+          <t>23966</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>53.25</v>
+        <v>49.37</v>
       </c>
       <c r="F53" t="n">
-        <v>54.9</v>
+        <v>50.9</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/creatina-fuel-150gr-iridium/p</t>
+          <t>https://www.farmaponte.com.br/creatina-90gr-atlas/p</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>7899732113873</t>
+          <t>7899732112159</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>Iridium</t>
+          <t>Sem marca</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Creatina 90Gr Atlas</t>
+          <t>Whey Wcp Concentrado Doce Leite 900Gr Iridium</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C54" t="n">
-        <v>56.56</v>
+        <v>157.12</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>23966</t>
+          <t>23973</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>49.37</v>
+        <v>145.39</v>
       </c>
       <c r="F54" t="n">
-        <v>50.9</v>
+        <v>149.89</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/creatina-90gr-atlas/p</t>
+          <t>https://www.farmaponte.com.br/whey-wcp-concentrado-doce-leite-900gr-iridium/p</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>7899732112159</t>
+          <t>7899732112142</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Sem marca</t>
+          <t>Iridium</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Whey Wcp Concentrado Doce Leite 900Gr Iridium</t>
+          <t>Whey 100  Pote Baunilha 900GR Integralmedica</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C55" t="n">
-        <v>157.12</v>
+        <v>184.44</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>23973</t>
+          <t>23836</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>145.39</v>
+        <v>161.02</v>
       </c>
       <c r="F55" t="n">
-        <v>149.89</v>
+        <v>166</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-wcp-concentrado-doce-leite-900gr-iridium/p</t>
+          <t>https://www.farmaponte.com.br/whey-100-pote-baunilha-900gr-integralmedica/p</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>7899732112142</t>
+          <t>7896311709984</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Iridium</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Whey 100  Pote Baunilha 900GR Integralmedica</t>
+          <t>Suplemento para Nutrição Nutren Control Diet chocolate, garrafa com 200mL</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>184.44</v>
+        <v>14.99</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>23836</t>
+          <t>20792</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>161.02</v>
+        <v>14.54</v>
       </c>
       <c r="F56" t="n">
-        <v>166</v>
+        <v>14.99</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-100-pote-baunilha-900gr-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/suplemento-alimentar-nutren-control-chocolate-200ml/p</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>7896311709984</t>
+          <t>7891000334133</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Nutren</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Suplemento para Nutrição Nutren Control Diet chocolate, garrafa com 200mL</t>
+          <t>Therma Pro Hardcore Com 60 Cápsulas Integralmedica</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>14.99</v>
+        <v>73.33</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>20792</t>
+          <t>24798</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>14.54</v>
+        <v>64.02</v>
       </c>
       <c r="F57" t="n">
-        <v>14.99</v>
+        <v>66</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/suplemento-alimentar-nutren-control-chocolate-200ml/p</t>
+          <t>https://www.farmaponte.com.br/therma-pro-hardcore-com-60-capsulas-integralmedica/p</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>7891000334133</t>
+          <t>7896311707973</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Nutren</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Therma Pro Hardcore Com 60 Cápsulas Integralmedica</t>
+          <t>Whey 100  Pote Chocolate 900GR Integralmedica</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>10</v>
       </c>
       <c r="C58" t="n">
-        <v>73.33</v>
+        <v>184.44</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>24798</t>
+          <t>23837</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>64.02</v>
+        <v>161.02</v>
       </c>
       <c r="F58" t="n">
-        <v>66</v>
+        <v>166</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/therma-pro-hardcore-com-60-capsulas-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/whey-100-pote-chocolate-900gr-integralmedica/p</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>7896311707973</t>
+          <t>7896311709991</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -2700,73 +2700,71 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Whey 100  Pote Chocolate 900GR Integralmedica</t>
+          <t>Fosfadil 30 cápsulas</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>184.44</v>
+        <v>78.75</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>23837</t>
+          <t>18729</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>161.02</v>
+        <v>76.39</v>
       </c>
       <c r="F59" t="n">
-        <v>166</v>
+        <v>78.75</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-100-pote-chocolate-900gr-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/fosfadil-30cps/p</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>7896311709991</t>
+          <t>7908135001554</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Sem marca</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Fosfadil 30 cápsulas</t>
+          <t>Kimera Thermo Iridium Labs 300mg 60 Comprimidos</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C60" t="n">
-        <v>78.75</v>
+        <v>79.12</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>18729</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
-        <v>76.39</v>
-      </c>
+          <t>25816</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="n">
-        <v>78.75</v>
+        <v>55.38</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/fosfadil-30cps/p</t>
+          <t>https://www.farmaponte.com.br/kimera-thermo-iridium-labs-300mg-60-comprimidos/p</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>7908135001554</t>
+          <t>7899732100323</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -2778,149 +2776,151 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Isotônico Powerade Limão 500ml</t>
+          <t>Bcaa 2400 90Caps Integralmédica</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>10</v>
       </c>
       <c r="C61" t="n">
-        <v>6.99</v>
+        <v>76.78</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>22732</t>
+          <t>23793</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>6.1</v>
+        <v>67.03</v>
       </c>
       <c r="F61" t="n">
-        <v>6.29</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/powerade-limao-500ml/p</t>
+          <t>https://www.farmaponte.com.br/bcaa-2400-90caps-integralmedica/p</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>7894900500035</t>
+          <t>7896311763269</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Powerade</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Isotônico Powerade Sabor Frutas Tropicais 500ml</t>
+          <t>Nutri Whey Refil Morango 900GR Integralmedica</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>6.99</v>
+        <v>102.43</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>24813</t>
+          <t>23832</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>6.1</v>
+        <v>89.42</v>
       </c>
       <c r="F62" t="n">
-        <v>6.29</v>
+        <v>92.19</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/isotonico-powerade-sabor-frutas-tropicais-500ml/p</t>
+          <t>https://www.farmaponte.com.br/nutri-whey-refil-morango-900gr-integralmedica/p</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>7894900508017</t>
+          <t>7896311709496</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Sem marca</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Kimera Thermo Iridium Labs 300mg 60 Comprimidos</t>
+          <t>Sinister Mass Chocolate 3KG Integralmedica</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>79.12</v>
+        <v>148.56</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>25816</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr"/>
+          <t>23834</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>129.69</v>
+      </c>
       <c r="F63" t="n">
-        <v>55.38</v>
+        <v>133.7</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/kimera-thermo-iridium-labs-300mg-60-comprimidos/p</t>
+          <t>https://www.farmaponte.com.br/mass-chocolate-3kg-integralmedica/p</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>7899732100323</t>
+          <t>7896311767298</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Sem marca</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Bcaa 2400 90Caps Integralmédica</t>
+          <t>Whey 100  Pote Morango 900GR Integralmedica</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>76.78</v>
+        <v>184.44</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>23793</t>
+          <t>23843</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>67.03</v>
+        <v>161.02</v>
       </c>
       <c r="F64" t="n">
-        <v>69.09999999999999</v>
+        <v>166</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/bcaa-2400-90caps-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/whey-100-pote-morango-900gr-integralmedica/p</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>7896311763269</t>
+          <t>7896311710010</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -2932,307 +2932,307 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Nutri Whey Refil Morango 900GR Integralmedica</t>
+          <t>Whey Protein Shake Dux Cookies 250ml</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>10</v>
       </c>
       <c r="C65" t="n">
-        <v>102.43</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>23832</t>
+          <t>24794</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>89.42</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="F65" t="n">
-        <v>92.19</v>
+        <v>8.9</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/nutri-whey-refil-morango-900gr-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/whey-protein-shake-dux-cookies-250ml/p</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>7896311709496</t>
+          <t>7898641074473</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Dux Nutrition</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Sinister Mass Chocolate 3KG Integralmedica</t>
+          <t>Whey Protein Shake Dux Chocolate 250Ml</t>
         </is>
       </c>
       <c r="B66" t="n">
         <v>10</v>
       </c>
       <c r="C66" t="n">
-        <v>148.56</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>23834</t>
+          <t>24795</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>129.69</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="F66" t="n">
-        <v>133.7</v>
+        <v>8.9</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/mass-chocolate-3kg-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/whey-protein-shake-dux-chocolate-250ml/p</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>7896311767298</t>
+          <t>7898641074497</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Dux Nutrition</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Whey 100  Pote Morango 900GR Integralmedica</t>
+          <t>Whey Protein Shake Dux Doce de Leite 250ml</t>
         </is>
       </c>
       <c r="B67" t="n">
         <v>10</v>
       </c>
       <c r="C67" t="n">
-        <v>184.44</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>23843</t>
+          <t>24792</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>161.02</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="F67" t="n">
-        <v>166</v>
+        <v>8.9</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-100-pote-morango-900gr-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/whey-protein-shake-dux-doce-de-leite-250ml/p</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>7896311710010</t>
+          <t>7898641074480</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Dux Nutrition</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Whey Protein Shake Dux Cookies 250ml</t>
+          <t>Suplemento Alimentar Florence Pro 6 Sachês de 4g cada</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C68" t="n">
-        <v>9.890000000000001</v>
+        <v>42.19</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>24794</t>
+          <t>23798</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>8.630000000000001</v>
+        <v>28.52</v>
       </c>
       <c r="F68" t="n">
-        <v>8.9</v>
+        <v>29.4</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-protein-shake-dux-cookies-250ml/p</t>
+          <t>https://www.farmaponte.com.br/suplemento-alimentar-florence-pro-6-saches-de-4g-cada-biolab/p</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>7898641074473</t>
+          <t>7896112407201</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>Dux Nutrition</t>
+          <t>Sem marca</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Whey Protein Shake Dux Chocolate 250Ml</t>
+          <t>Sinister Mass Baunilha 3KG Integralmedica</t>
         </is>
       </c>
       <c r="B69" t="n">
         <v>10</v>
       </c>
       <c r="C69" t="n">
-        <v>9.890000000000001</v>
+        <v>148.56</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>24795</t>
+          <t>23833</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>8.630000000000001</v>
+        <v>129.69</v>
       </c>
       <c r="F69" t="n">
-        <v>8.9</v>
+        <v>133.7</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-protein-shake-dux-chocolate-250ml/p</t>
+          <t>https://www.farmaponte.com.br/mass-baunilha-3kg-integralmedica/p</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>7898641074497</t>
+          <t>7896311767281</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>Dux Nutrition</t>
+          <t>Integralmédica</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Isotônico Powerade Mountain Blast 500ml</t>
+          <t>Whey Protein Dux Chocolate Branco 250ml</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>10</v>
       </c>
       <c r="C70" t="n">
-        <v>6.99</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>24783</t>
+          <t>24793</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>6.1</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="F70" t="n">
-        <v>6.29</v>
+        <v>8.9</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/isotonico-powerade-mountain-blast-500ml/p</t>
+          <t>https://www.farmaponte.com.br/whey-protein-dux-chocolate-branco-250ml/p</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>7894900504002</t>
+          <t>7898641074503</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>Sem marca</t>
+          <t>Dux Nutrition</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Whey Protein Shake Dux Doce de Leite 250ml</t>
+          <t>Isotônico Powerade Limão 500ml</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>10</v>
       </c>
       <c r="C71" t="n">
-        <v>9.890000000000001</v>
+        <v>6.99</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>24792</t>
+          <t>22732</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>8.630000000000001</v>
+        <v>6.1</v>
       </c>
       <c r="F71" t="n">
-        <v>8.9</v>
+        <v>6.29</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-protein-shake-dux-doce-de-leite-250ml/p</t>
+          <t>https://www.farmaponte.com.br/powerade-limao-500ml/p</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>7898641074480</t>
+          <t>7894900500035</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>Dux Nutrition</t>
+          <t>Powerade</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Suplemento Alimentar Florence Pro 6 Sachês de 4g cada</t>
+          <t>Isotônico Powerade Mountain Blast 500ml</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C72" t="n">
-        <v>42.19</v>
+        <v>6.99</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>23798</t>
+          <t>24783</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>28.52</v>
+        <v>6.1</v>
       </c>
       <c r="F72" t="n">
-        <v>29.4</v>
+        <v>6.29</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/suplemento-alimentar-florence-pro-6-saches-de-4g-cada-biolab/p</t>
+          <t>https://www.farmaponte.com.br/isotonico-powerade-mountain-blast-500ml/p</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>7896112407201</t>
+          <t>7894900504002</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -3244,78 +3244,78 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Sinister Mass Baunilha 3KG Integralmedica</t>
+          <t>Isotônico Powerade Sabor Frutas Tropicais 500ml</t>
         </is>
       </c>
       <c r="B73" t="n">
         <v>10</v>
       </c>
       <c r="C73" t="n">
-        <v>148.56</v>
+        <v>6.99</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>23833</t>
+          <t>24813</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>129.69</v>
+        <v>6.1</v>
       </c>
       <c r="F73" t="n">
-        <v>133.7</v>
+        <v>6.29</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/mass-baunilha-3kg-integralmedica/p</t>
+          <t>https://www.farmaponte.com.br/isotonico-powerade-sabor-frutas-tropicais-500ml/p</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>7896311767281</t>
+          <t>7894900508017</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>Integralmédica</t>
+          <t>Sem marca</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Whey Protein Dux Chocolate Branco 250ml</t>
+          <t>Go Energy Now Gel Guarana Com Acai 30gr</t>
         </is>
       </c>
       <c r="B74" t="n">
         <v>10</v>
       </c>
       <c r="C74" t="n">
-        <v>9.890000000000001</v>
+        <v>4.82</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>24793</t>
+          <t>25480</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>8.630000000000001</v>
+        <v>4.21</v>
       </c>
       <c r="F74" t="n">
-        <v>8.9</v>
+        <v>4.34</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.farmaponte.com.br/whey-protein-dux-chocolate-branco-250ml/p</t>
+          <t>https://www.farmaponte.com.br/go-energy-now-gel-guarana-com-acai-30gr/p</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>7898641074503</t>
+          <t>7899621106573</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>Dux Nutrition</t>
+          <t>Sem marca</t>
         </is>
       </c>
     </row>

</xml_diff>